<commit_message>
Created beautifull dashboard Give me my Money
</commit_message>
<xml_diff>
--- a/data/58. NUMBER OF TREKKERS IN DIFFERENT TREKKING AREA, 2001-2018..xlsx
+++ b/data/58. NUMBER OF TREKKERS IN DIFFERENT TREKKING AREA, 2001-2018..xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projekt\Nepal_Tourism_DashBoard\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projekt\Nepal_Tourism_DashBoard\New folder\Nepal_Tourism_DashBoard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C007FFF-F836-49F3-B1F4-9A01C902161E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC13139-461B-4902-ACC2-27CC594453DC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Year</t>
   </si>
@@ -74,15 +74,18 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF2B2A29"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -330,7 +333,7 @@
   <dimension ref="A1:V1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:V988"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -379,39 +382,17 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="1"/>
     </row>
     <row r="2" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
@@ -438,30 +419,14 @@
       <c r="K2" s="4">
         <v>3354</v>
       </c>
-      <c r="L2" s="3">
-        <v>2001</v>
-      </c>
-      <c r="M2" s="3">
-        <v>922</v>
-      </c>
-      <c r="N2" s="3">
-        <v>488</v>
-      </c>
-      <c r="O2" s="3">
-        <v>119</v>
-      </c>
-      <c r="P2" s="3">
-        <v>337</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>798</v>
-      </c>
-      <c r="R2" s="3">
-        <v>690</v>
-      </c>
-      <c r="V2" s="4">
-        <v>3354</v>
-      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="V2" s="4"/>
     </row>
     <row r="3" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
@@ -491,33 +456,15 @@
       <c r="K3" s="4">
         <v>1979</v>
       </c>
-      <c r="L3" s="3">
-        <v>2002</v>
-      </c>
-      <c r="M3" s="3">
-        <v>536</v>
-      </c>
-      <c r="N3" s="3">
-        <v>0</v>
-      </c>
-      <c r="O3" s="3">
-        <v>119</v>
-      </c>
-      <c r="P3" s="3">
-        <v>339</v>
-      </c>
-      <c r="Q3" s="3">
-        <v>428</v>
-      </c>
-      <c r="R3" s="3">
-        <v>478</v>
-      </c>
-      <c r="U3" s="3">
-        <v>79</v>
-      </c>
-      <c r="V3" s="4">
-        <v>1979</v>
-      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="4"/>
     </row>
     <row r="4" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
@@ -547,33 +494,15 @@
       <c r="K4" s="4">
         <v>2365</v>
       </c>
-      <c r="L4" s="3">
-        <v>2003</v>
-      </c>
-      <c r="M4" s="3">
-        <v>572</v>
-      </c>
-      <c r="N4" s="3">
-        <v>0</v>
-      </c>
-      <c r="O4" s="3">
-        <v>369</v>
-      </c>
-      <c r="P4" s="3">
-        <v>223</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>645</v>
-      </c>
-      <c r="R4" s="3">
-        <v>402</v>
-      </c>
-      <c r="U4" s="3">
-        <v>154</v>
-      </c>
-      <c r="V4" s="4">
-        <v>2365</v>
-      </c>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="4"/>
     </row>
     <row r="5" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
@@ -603,33 +532,15 @@
       <c r="K5" s="4">
         <v>3223</v>
       </c>
-      <c r="L5" s="3">
-        <v>2004</v>
-      </c>
-      <c r="M5" s="3">
-        <v>825</v>
-      </c>
-      <c r="N5" s="3">
-        <v>329</v>
-      </c>
-      <c r="O5" s="3">
-        <v>77</v>
-      </c>
-      <c r="P5" s="3">
-        <v>577</v>
-      </c>
-      <c r="Q5" s="3">
-        <v>682</v>
-      </c>
-      <c r="R5" s="3">
-        <v>458</v>
-      </c>
-      <c r="U5" s="3">
-        <v>275</v>
-      </c>
-      <c r="V5" s="4">
-        <v>3223</v>
-      </c>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="4"/>
     </row>
     <row r="6" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
@@ -659,33 +570,15 @@
       <c r="K6" s="4">
         <v>2714</v>
       </c>
-      <c r="L6" s="3">
-        <v>2005</v>
-      </c>
-      <c r="M6" s="3">
-        <v>661</v>
-      </c>
-      <c r="N6" s="3">
-        <v>200</v>
-      </c>
-      <c r="O6" s="3">
-        <v>81</v>
-      </c>
-      <c r="P6" s="3">
-        <v>782</v>
-      </c>
-      <c r="Q6" s="3">
-        <v>544</v>
-      </c>
-      <c r="R6" s="3">
-        <v>167</v>
-      </c>
-      <c r="U6" s="3">
-        <v>279</v>
-      </c>
-      <c r="V6" s="4">
-        <v>2714</v>
-      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="4"/>
     </row>
     <row r="7" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
@@ -715,33 +608,15 @@
       <c r="K7" s="4">
         <v>3112</v>
       </c>
-      <c r="L7" s="3">
-        <v>2006</v>
-      </c>
-      <c r="M7" s="3">
-        <v>248</v>
-      </c>
-      <c r="N7" s="3">
-        <v>225</v>
-      </c>
-      <c r="O7" s="3">
-        <v>92</v>
-      </c>
-      <c r="P7" s="4">
-        <v>1256</v>
-      </c>
-      <c r="Q7" s="3">
-        <v>561</v>
-      </c>
-      <c r="R7" s="3">
-        <v>335</v>
-      </c>
-      <c r="U7" s="3">
-        <v>395</v>
-      </c>
-      <c r="V7" s="4">
-        <v>3112</v>
-      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="4"/>
     </row>
     <row r="8" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
@@ -771,33 +646,15 @@
       <c r="K8" s="4">
         <v>5327</v>
       </c>
-      <c r="L8" s="3">
-        <v>2007</v>
-      </c>
-      <c r="M8" s="4">
-        <v>1282</v>
-      </c>
-      <c r="N8" s="3">
-        <v>419</v>
-      </c>
-      <c r="O8" s="3">
-        <v>198</v>
-      </c>
-      <c r="P8" s="4">
-        <v>1542</v>
-      </c>
-      <c r="Q8" s="3">
-        <v>895</v>
-      </c>
-      <c r="R8" s="3">
-        <v>404</v>
-      </c>
-      <c r="U8" s="3">
-        <v>587</v>
-      </c>
-      <c r="V8" s="4">
-        <v>5327</v>
-      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="4"/>
     </row>
     <row r="9" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
@@ -827,33 +684,15 @@
       <c r="K9" s="4">
         <v>6448</v>
       </c>
-      <c r="L9" s="3">
-        <v>2008</v>
-      </c>
-      <c r="M9" s="3">
-        <v>838</v>
-      </c>
-      <c r="N9" s="3">
-        <v>709</v>
-      </c>
-      <c r="O9" s="3">
-        <v>383</v>
-      </c>
-      <c r="P9" s="4">
-        <v>1065</v>
-      </c>
-      <c r="Q9" s="4">
-        <v>1443</v>
-      </c>
-      <c r="R9" s="4">
-        <v>1490</v>
-      </c>
-      <c r="U9" s="3">
-        <v>520</v>
-      </c>
-      <c r="V9" s="4">
-        <v>6448</v>
-      </c>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="4"/>
     </row>
     <row r="10" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
@@ -883,33 +722,15 @@
       <c r="K10" s="4">
         <v>6979</v>
       </c>
-      <c r="L10" s="3">
-        <v>2009</v>
-      </c>
-      <c r="M10" s="4">
-        <v>1659</v>
-      </c>
-      <c r="N10" s="3">
-        <v>739</v>
-      </c>
-      <c r="O10" s="3">
-        <v>313</v>
-      </c>
-      <c r="P10" s="4">
-        <v>1177</v>
-      </c>
-      <c r="Q10" s="4">
-        <v>1635</v>
-      </c>
-      <c r="R10" s="3">
-        <v>508</v>
-      </c>
-      <c r="U10" s="3">
-        <v>948</v>
-      </c>
-      <c r="V10" s="4">
-        <v>6979</v>
-      </c>
+      <c r="L10" s="3"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="4"/>
     </row>
     <row r="11" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
@@ -939,33 +760,15 @@
       <c r="K11" s="4">
         <v>9015</v>
       </c>
-      <c r="L11" s="3">
-        <v>2010</v>
-      </c>
-      <c r="M11" s="4">
-        <v>2162</v>
-      </c>
-      <c r="N11" s="3">
-        <v>785</v>
-      </c>
-      <c r="O11" s="3">
-        <v>358</v>
-      </c>
-      <c r="P11" s="4">
-        <v>1633</v>
-      </c>
-      <c r="Q11" s="4">
-        <v>2162</v>
-      </c>
-      <c r="R11" s="3">
-        <v>488</v>
-      </c>
-      <c r="U11" s="4">
-        <v>1427</v>
-      </c>
-      <c r="V11" s="4">
-        <v>9015</v>
-      </c>
+      <c r="L11" s="3"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="3"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
     </row>
     <row r="12" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
@@ -995,33 +798,15 @@
       <c r="K12" s="4">
         <v>10715</v>
       </c>
-      <c r="L12" s="3">
-        <v>2011</v>
-      </c>
-      <c r="M12" s="4">
-        <v>2950</v>
-      </c>
-      <c r="N12" s="3">
-        <v>808</v>
-      </c>
-      <c r="O12" s="3">
-        <v>397</v>
-      </c>
-      <c r="P12" s="4">
-        <v>1758</v>
-      </c>
-      <c r="Q12" s="4">
-        <v>2813</v>
-      </c>
-      <c r="R12" s="3">
-        <v>591</v>
-      </c>
-      <c r="U12" s="4">
-        <v>1398</v>
-      </c>
-      <c r="V12" s="4">
-        <v>10715</v>
-      </c>
+      <c r="L12" s="3"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="3"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
     </row>
     <row r="13" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
@@ -1057,39 +842,17 @@
       <c r="K13" s="4">
         <v>11632</v>
       </c>
-      <c r="L13" s="3">
-        <v>2012</v>
-      </c>
-      <c r="M13" s="4">
-        <v>2965</v>
-      </c>
-      <c r="N13" s="3">
-        <v>982</v>
-      </c>
-      <c r="O13" s="3">
-        <v>536</v>
-      </c>
-      <c r="P13" s="4">
-        <v>1508</v>
-      </c>
-      <c r="Q13" s="4">
-        <v>3319</v>
-      </c>
-      <c r="R13" s="3">
-        <v>635</v>
-      </c>
-      <c r="S13" s="3">
-        <v>780</v>
-      </c>
-      <c r="T13" s="3">
-        <v>515</v>
-      </c>
-      <c r="U13" s="3">
-        <v>392</v>
-      </c>
-      <c r="V13" s="4">
-        <v>11632</v>
-      </c>
+      <c r="L13" s="3"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="4"/>
     </row>
     <row r="14" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
@@ -1125,39 +888,17 @@
       <c r="K14" s="4">
         <v>12937</v>
       </c>
-      <c r="L14" s="3">
-        <v>2013</v>
-      </c>
-      <c r="M14" s="4">
-        <v>2862</v>
-      </c>
-      <c r="N14" s="3">
-        <v>585</v>
-      </c>
-      <c r="O14" s="3">
-        <v>338</v>
-      </c>
-      <c r="P14" s="4">
-        <v>1603</v>
-      </c>
-      <c r="Q14" s="4">
-        <v>4439</v>
-      </c>
-      <c r="R14" s="3">
-        <v>837</v>
-      </c>
-      <c r="S14" s="4">
-        <v>1179</v>
-      </c>
-      <c r="T14" s="3">
-        <v>862</v>
-      </c>
-      <c r="U14" s="3">
-        <v>232</v>
-      </c>
-      <c r="V14" s="4">
-        <v>12937</v>
-      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="4"/>
     </row>
     <row r="15" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
@@ -1193,39 +934,17 @@
       <c r="K15" s="3">
         <v>15065</v>
       </c>
-      <c r="L15" s="3">
-        <v>2014</v>
-      </c>
-      <c r="M15" s="3">
-        <v>3883</v>
-      </c>
-      <c r="N15" s="3">
-        <v>1117</v>
-      </c>
-      <c r="O15" s="3">
-        <v>469</v>
-      </c>
-      <c r="P15" s="3">
-        <v>492</v>
-      </c>
-      <c r="Q15" s="3">
-        <v>3764</v>
-      </c>
-      <c r="R15" s="3">
-        <v>777</v>
-      </c>
-      <c r="S15" s="3">
-        <v>1454</v>
-      </c>
-      <c r="T15" s="3">
-        <v>776</v>
-      </c>
-      <c r="U15" s="3">
-        <v>2333</v>
-      </c>
-      <c r="V15" s="3">
-        <v>15065</v>
-      </c>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
     </row>
     <row r="16" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
@@ -1261,39 +980,17 @@
       <c r="K16" s="3">
         <v>9679</v>
       </c>
-      <c r="L16" s="3">
-        <v>2015</v>
-      </c>
-      <c r="M16" s="3">
-        <v>2673</v>
-      </c>
-      <c r="N16" s="3">
-        <v>788</v>
-      </c>
-      <c r="O16" s="3">
-        <v>328</v>
-      </c>
-      <c r="P16" s="3">
-        <v>1346</v>
-      </c>
-      <c r="Q16" s="3">
-        <v>2134</v>
-      </c>
-      <c r="R16" s="3">
-        <v>731</v>
-      </c>
-      <c r="S16" s="3">
-        <v>636</v>
-      </c>
-      <c r="T16" s="3">
-        <v>770</v>
-      </c>
-      <c r="U16" s="3">
-        <v>273</v>
-      </c>
-      <c r="V16" s="3">
-        <v>9679</v>
-      </c>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
     </row>
     <row r="17" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
@@ -1329,39 +1026,17 @@
       <c r="K17" s="3">
         <v>23569</v>
       </c>
-      <c r="L17" s="3">
-        <v>2016</v>
-      </c>
-      <c r="M17" s="3">
-        <v>3984</v>
-      </c>
-      <c r="N17" s="3">
-        <v>1023</v>
-      </c>
-      <c r="O17" s="3">
-        <v>531</v>
-      </c>
-      <c r="P17" s="3">
-        <v>10105</v>
-      </c>
-      <c r="Q17" s="3">
-        <v>4650</v>
-      </c>
-      <c r="R17" s="3">
-        <v>502</v>
-      </c>
-      <c r="S17" s="3">
-        <v>1219</v>
-      </c>
-      <c r="T17" s="3">
-        <v>903</v>
-      </c>
-      <c r="U17" s="3">
-        <v>356</v>
-      </c>
-      <c r="V17" s="3">
-        <v>23569</v>
-      </c>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
     </row>
     <row r="18" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
@@ -1397,39 +1072,17 @@
       <c r="K18" s="3">
         <v>29993</v>
       </c>
-      <c r="L18" s="3">
-        <v>2017</v>
-      </c>
-      <c r="M18" s="3">
-        <v>4240</v>
-      </c>
-      <c r="N18" s="3">
-        <v>924</v>
-      </c>
-      <c r="O18" s="3">
-        <v>425</v>
-      </c>
-      <c r="P18" s="3">
-        <v>13398</v>
-      </c>
-      <c r="Q18" s="3">
-        <v>6632</v>
-      </c>
-      <c r="R18" s="3">
-        <v>479</v>
-      </c>
-      <c r="S18" s="3">
-        <v>1681</v>
-      </c>
-      <c r="T18" s="3">
-        <v>1115</v>
-      </c>
-      <c r="U18" s="3">
-        <v>1099</v>
-      </c>
-      <c r="V18" s="3">
-        <v>29993</v>
-      </c>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="3"/>
     </row>
     <row r="19" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
@@ -1465,39 +1118,17 @@
       <c r="K19" s="3">
         <v>28876</v>
       </c>
-      <c r="L19" s="3">
-        <v>2018</v>
-      </c>
-      <c r="M19" s="3">
-        <v>4116</v>
-      </c>
-      <c r="N19" s="3">
-        <v>1222</v>
-      </c>
-      <c r="O19" s="3">
-        <v>525</v>
-      </c>
-      <c r="P19" s="3">
-        <v>10814</v>
-      </c>
-      <c r="Q19" s="3">
-        <v>7371</v>
-      </c>
-      <c r="R19" s="3">
-        <v>970</v>
-      </c>
-      <c r="S19" s="3">
-        <v>2030</v>
-      </c>
-      <c r="T19" s="3">
-        <v>1291</v>
-      </c>
-      <c r="U19" s="3">
-        <v>537</v>
-      </c>
-      <c r="V19" s="3">
-        <v>28876</v>
-      </c>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
     </row>
     <row r="20" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>

</xml_diff>